<commit_message>
Se agrego codigo de prueba filtrado al principal
</commit_message>
<xml_diff>
--- a/out4.xlsx
+++ b/out4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1202,7 +1202,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>xe-0/0/36</t>
+          <t>xe-0/0/35</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1237,7 +1237,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>xe-0/0/37</t>
+          <t>xe-0/0/36</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>xe-0/0/38</t>
+          <t>xe-0/0/37</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1307,7 +1307,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>xe-0/0/39</t>
+          <t>xe-0/0/38</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1342,7 +1342,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>xe-0/0/40</t>
+          <t>xe-0/0/39</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1377,7 +1377,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>xe-0/0/41</t>
+          <t>xe-0/0/40</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1412,7 +1412,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>xe-0/0/42</t>
+          <t>xe-0/0/41</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1447,7 +1447,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>xe-0/0/43</t>
+          <t>xe-0/0/42</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1482,7 +1482,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>xe-0/0/44</t>
+          <t>xe-0/0/43</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1517,7 +1517,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>xe-0/0/45</t>
+          <t>xe-0/0/44</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1552,7 +1552,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>xe-0/0/46</t>
+          <t>xe-0/0/45</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1587,7 +1587,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>xe-0/0/47</t>
+          <t>xe-0/0/46</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1622,34 +1622,69 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
+        <v>1269</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>172.28.255.41</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MADRI-MADR-H-01-DAAS</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>xe-0/0/47</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PUERTOLIBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>1270</v>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>172.28.255.41</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>MADRI-MADR-H-01-DAAS</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>172.28.255.41</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MADRI-MADR-H-01-DAAS</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
         <is>
           <t>xe-0/0/48</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>PUERTOLIBRE</t>
         </is>

</xml_diff>